<commit_message>
table ss with pre-experiment data
</commit_message>
<xml_diff>
--- a/Tables/balance_response.xlsx
+++ b/Tables/balance_response.xlsx
@@ -1,31 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\xps-seira\Dropbox\Apps\ShareLaTeX\Donde2020\Tables\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90531B4D-4C7A-4628-AAF7-F1EAD1055654}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12600" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-23148" yWindow="-13068" windowWidth="23256" windowHeight="13176" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="exit" sheetId="5" r:id="rId1"/>
     <sheet name="basal" sheetId="3" r:id="rId2"/>
     <sheet name="balance_response" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="191029" fullCalcOnLoad="true"/>
 </workbook>
 </file>
 
@@ -50,9 +36,6 @@
     <t>Monday</t>
   </si>
   <si>
-    <t>Pawns</t>
-  </si>
-  <si>
     <t>Obs</t>
   </si>
   <si>
@@ -61,11 +44,14 @@
   <si>
     <t>Panel B : Exit Survey</t>
   </si>
+  <si>
+    <t>Number of branch-day pawns</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <fonts count="1">
     <font>
       <sz val="11"/>
@@ -162,37 +148,37 @@
   </cellStyleXfs>
   <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -201,14 +187,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -508,7 +486,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -517,93 +495,97 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
-    <row r="2" spans="2:5">
-      <c r="B2">
-        <v>2157.1458649015071</v>
-      </c>
-      <c r="C2">
+    <row r="2">
+      <c r="B2" s="0">
+        <v>2157.4058537363426</v>
+      </c>
+      <c r="C2" s="0">
         <v>2367.6243093922653</v>
       </c>
-      <c r="D2">
-        <v>2171.3144897351976</v>
-      </c>
-      <c r="E2">
-        <v>0.17174935988088755</v>
-      </c>
-    </row>
-    <row r="3" spans="2:5">
-      <c r="B3">
-        <v>30.927432150391382</v>
-      </c>
-      <c r="C3">
+      <c r="D2" s="0">
+        <v>2171.5569770901516</v>
+      </c>
+      <c r="E2" s="0">
+        <v>0.17228973589263194</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="B3" s="0">
+        <v>30.915340842769982</v>
+      </c>
+      <c r="C3" s="0">
         <v>154.83134488635548</v>
       </c>
-      <c r="D3">
-        <v>31.818971603836673</v>
-      </c>
-    </row>
-    <row r="4" spans="2:5">
-      <c r="B4">
-        <v>0.18239094026636893</v>
-      </c>
-      <c r="C4">
+      <c r="D3" s="0">
+        <v>31.807323205390613</v>
+      </c>
+      <c r="E3" s="0"/>
+    </row>
+    <row r="4">
+      <c r="B4" s="0">
+        <v>0.18231118909003907</v>
+      </c>
+      <c r="C4" s="0">
         <v>0.19337016574585636</v>
       </c>
-      <c r="D4">
-        <v>0.18313002082713478</v>
-      </c>
-      <c r="E4">
-        <v>0.7123917386381704</v>
-      </c>
-    </row>
-    <row r="5" spans="2:5">
-      <c r="B5">
-        <v>2.450518583303481E-2</v>
-      </c>
-      <c r="C5">
-        <v>3.6351262642859185E-2</v>
-      </c>
-      <c r="D5">
-        <v>2.4358084190383867E-2</v>
-      </c>
-    </row>
-    <row r="6" spans="2:5">
-      <c r="B6">
-        <v>32.830687830687829</v>
-      </c>
-      <c r="C6">
-        <v>35.655172413793103</v>
-      </c>
-      <c r="D6">
+      <c r="D4" s="0">
+        <v>0.18305563820291579</v>
+      </c>
+      <c r="E4" s="0">
+        <v>0.71034364024861918</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="B5" s="0">
+        <v>0.024499682973906006</v>
+      </c>
+      <c r="C5" s="0">
+        <v>0.036351262642859185</v>
+      </c>
+      <c r="D5" s="0">
+        <v>0.024353374831239075</v>
+      </c>
+      <c r="E5" s="0"/>
+    </row>
+    <row r="6">
+      <c r="B6" s="0">
+        <v>33.340425531914896</v>
+      </c>
+      <c r="C6" s="0">
+        <v>29.29032258064516</v>
+      </c>
+      <c r="D6" s="0">
         <v>33.031941031941031</v>
       </c>
-      <c r="E6">
-        <v>0.50668815294892589</v>
-      </c>
-    </row>
-    <row r="7" spans="2:5">
-      <c r="B7">
-        <v>1.0692588157130942</v>
-      </c>
-      <c r="C7">
-        <v>4.1754253675727302</v>
-      </c>
-      <c r="D7">
-        <v>1.0358452111568268</v>
-      </c>
-    </row>
-    <row r="8" spans="2:5">
-      <c r="B8">
+      <c r="E6" s="0">
+        <v>0.24593205180445749</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="B7" s="0">
+        <v>1.0865666714159887</v>
+      </c>
+      <c r="C7" s="0">
+        <v>3.3579286845159224</v>
+      </c>
+      <c r="D7" s="0">
+        <v>1.0362073711473245</v>
+      </c>
+      <c r="E7" s="0"/>
+    </row>
+    <row r="8">
+      <c r="B8" s="0">
         <v>12539</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="0">
         <v>905</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="0">
         <v>13444</v>
       </c>
-    </row>
-    <row r="9" spans="2:5">
+      <c r="E8" s="0"/>
+    </row>
+    <row r="9">
       <c r="B9">
         <v>0.4918311039287252</v>
       </c>
@@ -614,7 +596,7 @@
         <v>0.47863789777164084</v>
       </c>
     </row>
-    <row r="10" spans="2:5">
+    <row r="10">
       <c r="B10">
         <v>5740</v>
       </c>
@@ -631,7 +613,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -640,93 +622,97 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
-    <row r="2" spans="2:5">
-      <c r="B2">
-        <v>2194.854006968641</v>
-      </c>
-      <c r="C2">
-        <v>2153.7759605399792</v>
-      </c>
-      <c r="D2">
-        <v>2171.3144897351976</v>
-      </c>
-      <c r="E2">
-        <v>0.53323345837699354</v>
-      </c>
-    </row>
-    <row r="3" spans="2:5">
-      <c r="B3">
-        <v>50.164431495613719</v>
-      </c>
-      <c r="C3">
-        <v>41.805562372417199</v>
-      </c>
-      <c r="D3">
-        <v>31.818971603836669</v>
-      </c>
-    </row>
-    <row r="4" spans="2:5">
-      <c r="B4">
-        <v>0.18693379790940767</v>
-      </c>
-      <c r="C4">
-        <v>0.18029595015576325</v>
-      </c>
-      <c r="D4">
-        <v>0.18313002082713478</v>
-      </c>
-      <c r="E4">
-        <v>0.65842011749522522</v>
-      </c>
-    </row>
-    <row r="5" spans="2:5">
-      <c r="B5">
-        <v>2.4686198503598478E-2</v>
-      </c>
-      <c r="C5">
-        <v>2.6026371288691567E-2</v>
-      </c>
-      <c r="D5">
-        <v>2.4358084190383867E-2</v>
-      </c>
-    </row>
-    <row r="6" spans="2:5">
-      <c r="B6">
-        <v>30.907608695652176</v>
-      </c>
-      <c r="C6">
-        <v>34.784753363228702</v>
-      </c>
-      <c r="D6">
+    <row r="2">
+      <c r="B2" s="0">
+        <v>2262.1439973395409</v>
+      </c>
+      <c r="C2" s="0">
+        <v>2145.4579860113058</v>
+      </c>
+      <c r="D2" s="0">
+        <v>2171.5569770901516</v>
+      </c>
+      <c r="E2" s="0">
+        <v>0.077363019270749664</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="B3" s="0">
+        <v>59.211959578633127</v>
+      </c>
+      <c r="C3" s="0">
+        <v>35.445186055768197</v>
+      </c>
+      <c r="D3" s="0">
+        <v>31.80732320539061</v>
+      </c>
+      <c r="E3" s="0"/>
+    </row>
+    <row r="4">
+      <c r="B4" s="0">
+        <v>0.18190887928167609</v>
+      </c>
+      <c r="C4" s="0">
+        <v>0.18338603046852545</v>
+      </c>
+      <c r="D4" s="0">
+        <v>0.18305563820291579</v>
+      </c>
+      <c r="E4" s="0">
+        <v>0.94953992198672665</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="B5" s="0">
+        <v>0.031453663923441053</v>
+      </c>
+      <c r="C5" s="0">
+        <v>0.024509689361658406</v>
+      </c>
+      <c r="D5" s="0">
+        <v>0.024353374831239075</v>
+      </c>
+      <c r="E5" s="0"/>
+    </row>
+    <row r="6">
+      <c r="B6" s="0">
+        <v>32.127450980392155</v>
+      </c>
+      <c r="C6" s="0">
+        <v>33.334426229508196</v>
+      </c>
+      <c r="D6" s="0">
         <v>33.031941031941031</v>
       </c>
-      <c r="E6">
-        <v>5.6863052023573363E-2</v>
-      </c>
-    </row>
-    <row r="7" spans="2:5">
-      <c r="B7">
-        <v>1.3356266214626269</v>
-      </c>
-      <c r="C7">
-        <v>1.5288712643572433</v>
-      </c>
-      <c r="D7">
-        <v>1.0358452111568268</v>
-      </c>
-    </row>
-    <row r="8" spans="2:5">
-      <c r="B8">
-        <v>5740</v>
-      </c>
-      <c r="C8">
-        <v>7704</v>
-      </c>
-      <c r="D8">
+      <c r="E6" s="0">
+        <v>0.61423991149630908</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="B7" s="0">
+        <v>2.0762812455551489</v>
+      </c>
+      <c r="C7" s="0">
+        <v>1.1972335117199615</v>
+      </c>
+      <c r="D7" s="0">
+        <v>1.0362073711473245</v>
+      </c>
+      <c r="E7" s="0"/>
+    </row>
+    <row r="8">
+      <c r="B8" s="0">
+        <v>3007</v>
+      </c>
+      <c r="C8" s="0">
+        <v>10437</v>
+      </c>
+      <c r="D8" s="0">
         <v>13444</v>
       </c>
-    </row>
-    <row r="9" spans="2:5">
+      <c r="E8" s="0"/>
+    </row>
+    <row r="9">
       <c r="B9">
         <v>0.4918311039287252</v>
       </c>
@@ -737,7 +723,7 @@
         <v>0.47863789777164084</v>
       </c>
     </row>
-    <row r="10" spans="2:5">
+    <row r="10">
       <c r="B10">
         <v>5740</v>
       </c>
@@ -754,38 +740,38 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:I14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="A2:H10"/>
+    <sheetView tabSelected="true" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="12.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.44140625" bestFit="true" customWidth="true"/>
     <col min="2" max="2" width="8.88671875" style="4"/>
-    <col min="3" max="3" width="12" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12" style="4" bestFit="true" customWidth="true"/>
     <col min="4" max="4" width="8.88671875" style="4"/>
-    <col min="5" max="5" width="7" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7" style="4" bestFit="true" customWidth="true"/>
+    <col min="6" max="6" width="11.6640625" bestFit="true" customWidth="true"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:9" ht="15" thickBot="1">
+    <row r="2" ht="15" thickBot="true">
       <c r="A2" s="2"/>
       <c r="B2" s="7"/>
       <c r="C2" s="13" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D2" s="13"/>
       <c r="E2" s="13"/>
       <c r="F2" s="12" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G2" s="13"/>
       <c r="H2" s="13"/>
     </row>
-    <row r="3" spans="1:9" ht="15.6" thickTop="1" thickBot="1">
+    <row r="3" ht="15.6" thickTop="true" thickBot="true">
       <c r="A3" s="1"/>
       <c r="B3" s="5" t="s">
         <v>0</v>
@@ -809,7 +795,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="15" thickTop="1">
+    <row r="4" ht="15" thickTop="true">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -842,7 +828,7 @@
         <v>0.17</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5">
       <c r="B5" s="4" t="str">
         <f>CONCATENATE("(",ROUND(basal!D3,2),")")</f>
         <v>(31.82)</v>
@@ -865,7 +851,7 @@
       </c>
       <c r="H5" s="4"/>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -898,7 +884,7 @@
         <v>0.71</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7">
       <c r="A7" s="3"/>
       <c r="B7" s="6" t="str">
         <f>CONCATENATE("(",ROUND(basal!D5,2),")")</f>
@@ -922,9 +908,9 @@
       </c>
       <c r="H7" s="4"/>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8">
       <c r="A8" s="3" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B8" s="6">
         <f>ROUND(basal!D6,2)</f>
@@ -955,7 +941,7 @@
         <v>0.51</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9">
       <c r="A9" s="3"/>
       <c r="B9" s="6" t="str">
         <f>CONCATENATE("(",ROUND(basal!D7,2),")")</f>
@@ -980,9 +966,9 @@
       </c>
       <c r="H9" s="6"/>
     </row>
-    <row r="10" spans="1:9" ht="15" thickBot="1">
+    <row r="10" ht="15" thickBot="true">
       <c r="A10" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B10" s="7">
         <f>basal!D8</f>
@@ -1007,8 +993,8 @@
       </c>
       <c r="H10" s="7"/>
     </row>
-    <row r="11" spans="1:9" ht="15" thickTop="1"/>
-    <row r="14" spans="1:9">
+    <row r="11" ht="15" thickTop="true"/>
+    <row r="14">
       <c r="F14" s="4"/>
       <c r="G14" s="4"/>
       <c r="H14" s="4"/>

</xml_diff>